<commit_message>
Minor changes to v0.3.2 BOM
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.3/v0.3.2_bom.xlsx
+++ b/reference/hardware/v0.3/v0.3.2_bom.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/speeduino/reference/hardware/v0.3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/reference/hardware/v0.3/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full Kit" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2 Channel'!$A$1:$P$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Full Kit'!$A$1:$P$51</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="211">
   <si>
     <t>QTY</t>
   </si>
@@ -233,18 +234,12 @@
     <t>10k</t>
   </si>
   <si>
-    <t>RES 10.0K OHM 1/4W 1% METAL FILM</t>
-  </si>
-  <si>
     <t>Yageo</t>
   </si>
   <si>
     <t>MFR-25FBF-10K0</t>
   </si>
   <si>
-    <t>10.0KXBK-ND</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
@@ -729,6 +724,12 @@
   </si>
   <si>
     <t>R39, 40,54</t>
+  </si>
+  <si>
+    <t>10KQBK-ND</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1/4W 5% AXIAL</t>
   </si>
 </sst>
 </file>
@@ -736,7 +737,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -977,10 +978,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -998,7 +999,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1007,7 +1008,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1033,7 +1034,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1443,10 +1444,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1462,12 +1463,12 @@
     <col min="16" max="16" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1479,7 +1480,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -1488,7 +1489,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -1506,10 +1507,10 @@
         <v>10</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1542,13 +1543,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -1561,13 +1562,13 @@
         <v>16</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L3" s="5">
         <v>1.7</v>
@@ -1578,7 +1579,7 @@
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4" t="str">
-        <f t="shared" ref="O3:O50" si="1">IF(NOT(K3=""),A3&amp;","&amp;K3,"")</f>
+        <f t="shared" ref="O3:O49" si="1">IF(NOT(K3=""),A3&amp;","&amp;K3,"")</f>
         <v>1,399-3654-ND</v>
       </c>
       <c r="P3" t="str">
@@ -1592,13 +1593,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>15</v>
@@ -1611,13 +1612,13 @@
         <v>16</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L4" s="5">
         <v>0.66</v>
@@ -1642,13 +1643,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
@@ -1661,13 +1662,13 @@
         <v>16</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L5" s="5">
         <v>0.32</v>
@@ -1692,13 +1693,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
@@ -1711,13 +1712,13 @@
         <v>16</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L6" s="5">
         <v>1.57</v>
@@ -1742,13 +1743,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>15</v>
@@ -1761,13 +1762,13 @@
         <v>13</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L7" s="5">
         <v>0.62</v>
@@ -1792,13 +1793,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>15</v>
@@ -1811,13 +1812,13 @@
         <v>16</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L8" s="5">
         <v>0.24</v>
@@ -1842,13 +1843,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>15</v>
@@ -1861,13 +1862,13 @@
         <v>16</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="L9" s="5">
         <v>0.66</v>
@@ -1892,13 +1893,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>15</v>
@@ -1909,13 +1910,13 @@
         <v>16</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L10" s="5">
         <v>0.25</v>
@@ -1980,10 +1981,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>22</v>
@@ -1999,7 +2000,7 @@
         <v>24</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>25</v>
@@ -2030,10 +2031,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>28</v>
@@ -2049,7 +2050,7 @@
         <v>29</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>27</v>
@@ -2080,26 +2081,26 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L15" s="5">
         <v>0.47</v>
@@ -2124,7 +2125,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>32</v>
@@ -2143,7 +2144,7 @@
         <v>29</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>34</v>
@@ -2188,7 +2189,7 @@
         <v/>
       </c>
       <c r="P17" t="str">
-        <f t="shared" ref="P17:P45" si="5">A17&amp;"x "&amp;C17</f>
+        <f t="shared" ref="P17:P44" si="5">A17&amp;"x "&amp;C17</f>
         <v xml:space="preserve">x </v>
       </c>
     </row>
@@ -2245,7 +2246,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>36</v>
@@ -2264,7 +2265,7 @@
         <v>39</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>40</v>
@@ -2318,28 +2319,28 @@
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L22" s="3">
         <v>0.40200000000000002</v>
@@ -2349,7 +2350,7 @@
         <v>5.6280000000000001</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O22" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2365,24 +2366,24 @@
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L23" s="5">
         <v>0.1</v>
@@ -2406,13 +2407,13 @@
         <v>2</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -2420,16 +2421,16 @@
         <v>1</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L24" s="6">
         <v>0.56000000000000005</v>
@@ -2502,16 +2503,16 @@
         <v>8</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3">
@@ -2521,13 +2522,13 @@
         <v>43</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L27" s="6">
         <v>1.51</v>
@@ -2592,13 +2593,13 @@
         <v>3</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>45</v>
+        <v>210</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -2606,16 +2607,16 @@
         <v>7</v>
       </c>
       <c r="H30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I30" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="K30" s="2" t="s">
-        <v>48</v>
+        <v>209</v>
       </c>
       <c r="L30" s="5">
         <v>0.08</v>
@@ -2627,7 +2628,7 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>3,10.0KXBK-ND</v>
+        <v>3,10KQBK-ND</v>
       </c>
       <c r="P30" t="str">
         <f>"Resistor - " &amp; A30&amp;"x "&amp;C30</f>
@@ -2640,13 +2641,13 @@
         <v>12</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -2654,16 +2655,16 @@
         <v>32</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L31" s="5">
         <v>0.06</v>
@@ -2688,26 +2689,26 @@
         <v>8</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C32" s="14">
         <v>680</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L32" s="15">
         <v>0.22</v>
@@ -2717,7 +2718,7 @@
         <v>1.76</v>
       </c>
       <c r="N32" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="O32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2734,13 +2735,13 @@
         <v>6</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C33" s="3">
         <v>470</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -2748,16 +2749,16 @@
         <v>9</v>
       </c>
       <c r="H33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="L33" s="5">
         <v>0.11</v>
@@ -2781,32 +2782,32 @@
         <v>2</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3">
         <v>3</v>
       </c>
       <c r="H34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K34" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="L34" s="5">
         <v>1.92</v>
@@ -2830,13 +2831,13 @@
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -2844,16 +2845,16 @@
         <v>1</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L35" s="5">
         <v>0.46</v>
@@ -2863,7 +2864,7 @@
         <v>0.46</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O35" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2879,13 +2880,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -2893,16 +2894,16 @@
         <v>1</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L36" s="5">
         <v>0.46</v>
@@ -2912,7 +2913,7 @@
         <v>0.46</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O36" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2929,13 +2930,13 @@
         <v>12</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -2943,16 +2944,16 @@
         <v>17</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L37" s="5">
         <v>0.1</v>
@@ -2977,13 +2978,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C38" s="3">
         <v>160</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -2991,16 +2992,16 @@
         <v>4</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L38" s="5">
         <v>0.27</v>
@@ -3064,32 +3065,32 @@
         <v>1</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3">
         <v>2</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L41" s="5">
         <v>1.68</v>
@@ -3113,28 +3114,28 @@
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3">
         <v>1</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L42" s="6">
         <v>15.41</v>
@@ -3158,30 +3159,30 @@
         <v>2</v>
       </c>
       <c r="B43" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="E43" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="14">
         <v>2</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J43" s="14"/>
       <c r="K43" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L43" s="25">
         <v>2.92</v>
@@ -3200,110 +3201,90 @@
         <v>2x TC4424EPA</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="21">
-        <v>1</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>112</v>
+        <v>3</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>102</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>139</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="H44" s="3"/>
       <c r="I44" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="L44" s="6">
-        <v>1.61</v>
+        <v>0.5</v>
       </c>
       <c r="M44" s="6">
         <f>L44*A44</f>
-        <v>1.61</v>
-      </c>
-      <c r="N44" s="4" t="s">
-        <v>136</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="N44" s="4"/>
       <c r="O44" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>1,24LC512-I/P-ND</v>
+        <v>3,AE10011-ND</v>
       </c>
       <c r="P44" t="str">
         <f t="shared" si="5"/>
-        <v>1x 512Kb EEPROM</v>
+        <v>3x IC Socket</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="21">
-        <v>3</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>160</v>
-      </c>
+      <c r="A45" s="18"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="L45" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="M45" s="6">
-        <f>L45*A45</f>
-        <v>1.5</v>
-      </c>
-      <c r="N45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
       <c r="O45" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>3,AE10011-ND</v>
-      </c>
-      <c r="P45" t="str">
-        <f t="shared" si="5"/>
-        <v>3x IC Socket</v>
+        <v/>
       </c>
     </row>
     <row r="46" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="18">
+        <v>0</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="11"/>
+      <c r="G46" s="3">
+        <v>1</v>
+      </c>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6">
+        <f>L46*A46</f>
+        <v>0</v>
+      </c>
       <c r="N46" s="11"/>
       <c r="O46" s="4" t="str">
         <f t="shared" si="1"/>
@@ -3311,28 +3292,19 @@
       </c>
     </row>
     <row r="47" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18">
-        <v>0</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>118</v>
-      </c>
+      <c r="A47" s="18"/>
+      <c r="B47" s="4"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="3">
-        <v>1</v>
-      </c>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6">
-        <f>L47*A47</f>
-        <v>0</v>
-      </c>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="11"/>
       <c r="N47" s="11"/>
       <c r="O47" s="4" t="str">
         <f t="shared" si="1"/>
@@ -3341,40 +3313,57 @@
     </row>
     <row r="48" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
-      <c r="B48" s="4"/>
+      <c r="B48" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="4"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="9"/>
       <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="10"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="4"/>
       <c r="K48" s="3"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="4"/>
       <c r="O48" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
+      <c r="A49" s="18">
+        <v>1</v>
+      </c>
       <c r="B49" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="3"/>
+        <v>121</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="4"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="K49" s="3"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="3"/>
+      <c r="L49" s="6">
+        <v>15</v>
+      </c>
+      <c r="M49" s="6">
+        <f>L49*A49</f>
+        <v>15</v>
+      </c>
       <c r="N49" s="4"/>
       <c r="O49" s="4" t="str">
         <f t="shared" si="1"/>
@@ -3386,99 +3375,63 @@
         <v>1</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>85</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="3">
-        <v>1</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
       <c r="I50" s="3"/>
-      <c r="J50" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K50" s="3"/>
-      <c r="L50" s="6">
-        <v>15</v>
-      </c>
-      <c r="M50" s="6">
-        <f>L50*A50</f>
-        <v>15</v>
-      </c>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L50" s="3">
+        <v>61.65</v>
+      </c>
+      <c r="M50" s="6"/>
+      <c r="N50" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18">
-        <v>1</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>116</v>
-      </c>
+      <c r="A51" s="18"/>
+      <c r="B51" s="4"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="L51" s="3">
-        <v>61.65</v>
-      </c>
-      <c r="M51" s="6"/>
-      <c r="N51" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="K52" s="30"/>
-      <c r="L52" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M52" s="12">
-        <f>SUM(M2:M51)</f>
-        <v>92.628</v>
-      </c>
-      <c r="N52" s="11" t="s">
-        <v>83</v>
+      <c r="F51" s="26"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="K51" s="30"/>
+      <c r="L51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M51" s="12">
+        <f>SUM(M2:M50)</f>
+        <v>91.018000000000001</v>
+      </c>
+      <c r="N51" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P51"/>
   <mergeCells count="1">
-    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="J51:K51"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K6" r:id="rId1" display="478-1910-ND"/>
     <hyperlink ref="K14" r:id="rId2"/>
     <hyperlink ref="K20" r:id="rId3"/>
-    <hyperlink ref="K30" r:id="rId4"/>
+    <hyperlink ref="K30" r:id="rId4" display="10.0KXBK-ND"/>
     <hyperlink ref="K34" r:id="rId5"/>
     <hyperlink ref="K35" r:id="rId6"/>
     <hyperlink ref="K36" r:id="rId7"/>
@@ -3496,13 +3449,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3520,12 +3473,12 @@
     <col min="16" max="16" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -3537,13 +3490,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -3564,10 +3517,10 @@
         <v>10</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3600,13 +3553,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -3616,16 +3569,16 @@
         <v>4</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L3" s="5">
         <v>1.7</v>
@@ -3650,13 +3603,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>15</v>
@@ -3666,16 +3619,16 @@
         <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L4" s="5">
         <v>0.66</v>
@@ -3700,13 +3653,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
@@ -3716,16 +3669,16 @@
         <v>17</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L5" s="5">
         <v>0.32</v>
@@ -3750,13 +3703,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
@@ -3766,16 +3719,16 @@
         <v>2</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L6" s="5">
         <v>1.57</v>
@@ -3800,13 +3753,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>15</v>
@@ -3816,16 +3769,16 @@
         <v>2</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L7" s="5">
         <v>0.62</v>
@@ -3850,13 +3803,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>15</v>
@@ -3866,16 +3819,16 @@
         <v>3</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L8" s="5">
         <v>0.24</v>
@@ -3900,13 +3853,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>15</v>
@@ -3916,16 +3869,16 @@
         <v>4</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="L9" s="5">
         <v>0.66</v>
@@ -3950,13 +3903,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>15</v>
@@ -3964,16 +3917,16 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L10" s="5">
         <v>0.25</v>
@@ -4038,10 +3991,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>22</v>
@@ -4054,7 +4007,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>24</v>
@@ -4082,16 +4035,16 @@
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>28</v>
@@ -4104,7 +4057,7 @@
         <v>18</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>29</v>
@@ -4132,32 +4085,32 @@
         <v>Diode - 12x 1N5818-TP Schottky</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
         <v>4</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L15" s="5">
         <v>0.47</v>
@@ -4182,7 +4135,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>32</v>
@@ -4198,7 +4151,7 @@
         <v>13</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>29</v>
@@ -4303,7 +4256,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>36</v>
@@ -4319,7 +4272,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>39</v>
@@ -4371,33 +4324,33 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L22" s="3">
         <v>0.40200000000000002</v>
@@ -4407,7 +4360,7 @@
         <v>5.6280000000000001</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O22" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4418,29 +4371,29 @@
         <v>14x Dual Terminal Block</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L23" s="5">
         <v>0.1</v>
@@ -4459,18 +4412,18 @@
         <v>5x Jumper</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>2</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -4478,16 +4431,16 @@
         <v>1</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L24" s="6">
         <v>0.56000000000000005</v>
@@ -4559,32 +4512,32 @@
         <v>6</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3">
         <v>8</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>43</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L27" s="6">
         <v>1.51</v>
@@ -4649,13 +4602,13 @@
         <v>3</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>45</v>
+        <v>210</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -4663,16 +4616,16 @@
         <v>7</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J30" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="K30" s="2" t="s">
-        <v>48</v>
+        <v>209</v>
       </c>
       <c r="L30" s="5">
         <v>0.08</v>
@@ -4684,7 +4637,7 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>3,10.0KXBK-ND</v>
+        <v>3,10KQBK-ND</v>
       </c>
       <c r="P30" t="str">
         <f>"Resistor - " &amp; A30&amp;"x "&amp;C30</f>
@@ -4697,13 +4650,13 @@
         <v>8</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -4711,16 +4664,16 @@
         <v>32</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L31" s="5">
         <v>0.06</v>
@@ -4745,26 +4698,26 @@
         <v>4</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C32" s="14">
         <v>680</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L32" s="15">
         <v>0.22</v>
@@ -4774,7 +4727,7 @@
         <v>0.88</v>
       </c>
       <c r="N32" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="O32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4791,13 +4744,13 @@
         <v>6</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C33" s="3">
         <v>470</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -4805,16 +4758,16 @@
         <v>9</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="L33" s="5">
         <v>0.11</v>
@@ -4839,32 +4792,32 @@
         <v>2</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3">
         <v>3</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K34" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="L34" s="5">
         <v>1.92</v>
@@ -4888,13 +4841,13 @@
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -4902,16 +4855,16 @@
         <v>1</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L35" s="5">
         <v>0.46</v>
@@ -4921,7 +4874,7 @@
         <v>0.46</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O35" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4937,13 +4890,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -4951,16 +4904,16 @@
         <v>1</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L36" s="5">
         <v>0.46</v>
@@ -4970,7 +4923,7 @@
         <v>0.46</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O36" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4987,13 +4940,13 @@
         <v>8</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -5001,16 +4954,16 @@
         <v>17</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L37" s="5">
         <v>0.1</v>
@@ -5034,13 +4987,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C38" s="3">
         <v>160</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -5048,16 +5001,16 @@
         <v>4</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L38" s="5">
         <v>0.27</v>
@@ -5121,32 +5074,32 @@
         <v>1</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3">
         <v>2</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L41" s="5">
         <v>1.68</v>
@@ -5170,16 +5123,16 @@
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3">
@@ -5187,11 +5140,11 @@
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L42" s="6">
         <v>15.41</v>
@@ -5215,30 +5168,30 @@
         <v>1</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C43" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="14">
         <v>2</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J43" s="14"/>
       <c r="K43" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L43" s="25">
         <v>2.92</v>
@@ -5262,30 +5215,30 @@
         <v>1</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L44" s="6">
         <v>1.61</v>
@@ -5295,7 +5248,7 @@
         <v>1.61</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O44" s="4" t="str">
         <f t="shared" si="1"/>
@@ -5311,24 +5264,24 @@
         <v>3</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L45" s="6">
         <v>0.5</v>
@@ -5372,7 +5325,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -5419,7 +5372,7 @@
     <row r="49" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -5443,10 +5396,10 @@
         <v>1</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -5456,10 +5409,10 @@
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K50" s="3"/>
       <c r="L50" s="6">
@@ -5480,7 +5433,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -5491,14 +5444,14 @@
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L51" s="3">
         <v>61.65</v>
       </c>
       <c r="M51" s="6"/>
       <c r="N51" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5512,22 +5465,28 @@
       <c r="H52" s="9"/>
       <c r="I52" s="4"/>
       <c r="J52" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K52" s="30"/>
       <c r="L52" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M52" s="12">
         <f>SUM(M2:M51)</f>
         <v>80.698000000000008</v>
       </c>
       <c r="N52" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P52"/>
+  <autoFilter ref="A1:P52">
+    <filterColumn colId="7">
+      <filters blank="1">
+        <filter val="Y"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="J52:K52"/>
   </mergeCells>
@@ -5538,7 +5497,7 @@
     <hyperlink ref="K8" r:id="rId3" display="399-4148-ND"/>
     <hyperlink ref="K14" r:id="rId4"/>
     <hyperlink ref="K20" r:id="rId5"/>
-    <hyperlink ref="K30" r:id="rId6"/>
+    <hyperlink ref="K30" r:id="rId6" display="10.0KXBK-ND"/>
     <hyperlink ref="K34" r:id="rId7"/>
     <hyperlink ref="K35" r:id="rId8"/>
     <hyperlink ref="K36" r:id="rId9"/>

</xml_diff>

<commit_message>
Minor BOM update to v0.3.2
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.3/v0.3.2_bom.xlsx
+++ b/reference/hardware/v0.3/v0.3.2_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="203">
   <si>
     <t>QTY</t>
   </si>
@@ -694,6 +694,18 @@
   </si>
   <si>
     <t>R10,13,16,19,21,23,24,29,30,50,51,57,58</t>
+  </si>
+  <si>
+    <t>PPC2.49KXCT-ND</t>
+  </si>
+  <si>
+    <t>RES 2.49K OHM 1/2W 1% AXIAL</t>
+  </si>
+  <si>
+    <t>Vishay BC Components</t>
+  </si>
+  <si>
+    <t>SFR16S0002491FR500</t>
   </si>
 </sst>
 </file>
@@ -1399,13 +1411,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1471,7 +1483,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -1495,7 +1507,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
@@ -1545,7 +1557,7 @@
         <v>Capacitor - 1x 10uF</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <f>LEN(B4)-LEN(SUBSTITUTE(B4,",",""))+1</f>
         <v>5</v>
@@ -1595,7 +1607,7 @@
         <v>Capacitor - 5x 0.22uF</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
         <v>7</v>
@@ -1645,7 +1657,7 @@
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
         <v>1</v>
@@ -1695,7 +1707,7 @@
         <v>Capacitor - 1x 47uF</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <f t="shared" ref="A7:A9" si="3">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
         <v>1</v>
@@ -1745,7 +1757,7 @@
         <v>Capacitor - 1x 0.33uF</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -1795,7 +1807,7 @@
         <v>Capacitor - 1x 0.01uF</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -1845,7 +1857,7 @@
         <v>Capacitor - 3x 1uF</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
         <v>1</v>
@@ -1893,7 +1905,7 @@
         <v>Capacitor - 1x 4.7nF</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -1913,7 +1925,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
@@ -1933,7 +1945,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="40" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
         <v>1</v>
@@ -1983,7 +1995,7 @@
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="40" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>12</v>
@@ -2008,7 +2020,7 @@
         <v>29</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>27</v>
@@ -2077,7 +2089,7 @@
         <v>Diode - 8x LED-Red</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="40" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
         <v>4</v>
@@ -2127,7 +2139,7 @@
         <v>Diode - 4x 1N4004</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
@@ -2151,7 +2163,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>1</v>
       </c>
@@ -2200,7 +2212,7 @@
         <v>1x Surge Protection</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
@@ -2359,7 +2371,7 @@
         <v>5x 40 POS 0.100 Pin Header</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
@@ -2383,7 +2395,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
@@ -2407,7 +2419,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <f>LEN(B25)-LEN(SUBSTITUTE(B25,",",""))+1</f>
         <v>8</v>
@@ -2457,7 +2469,7 @@
         <v>8x 62A MOSFET N-CH</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
@@ -2477,7 +2489,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
@@ -2497,7 +2509,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <f>LEN(B28)-LEN(SUBSTITUTE(B28,",",""))+1</f>
         <v>3</v>
@@ -2545,7 +2557,7 @@
         <v>Resistor - 3x 10k</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
         <f>LEN(B29)-LEN(SUBSTITUTE(B29,",",""))+1</f>
         <v>13</v>
@@ -2593,7 +2605,7 @@
         <v>Resistor - 13x 1k</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
         <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
         <v>8</v>
@@ -2639,7 +2651,7 @@
         <v>Resistor - 8x 680</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="40" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
         <v>6</v>
@@ -2687,7 +2699,7 @@
         <v>Resistor - 6x 470</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
         <v>2</v>
       </c>
@@ -2698,7 +2710,7 @@
         <v>149</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>55</v>
+        <v>200</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>56</v>
@@ -2708,16 +2720,16 @@
         <v>3</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>57</v>
+        <v>201</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>192</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>58</v>
+        <v>202</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>59</v>
+        <v>199</v>
       </c>
       <c r="L32" s="5">
         <v>1.92</v>
@@ -2729,14 +2741,14 @@
       <c r="N32" s="4"/>
       <c r="O32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>2,985-1047-1-ND</v>
+        <v>2,PPC2.49KXCT-ND</v>
       </c>
       <c r="P32" t="str">
         <f t="shared" si="7"/>
         <v>Resistor - 2x 0.1% 2.49k</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
         <v>1</v>
       </c>
@@ -2767,11 +2779,11 @@
         <v>62</v>
       </c>
       <c r="L33" s="5">
-        <v>0.46</v>
+        <v>0.3</v>
       </c>
       <c r="M33" s="6">
         <f t="shared" si="6"/>
-        <v>0.46</v>
+        <v>0.3</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>119</v>
@@ -2785,7 +2797,7 @@
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
         <f t="shared" ref="A34:A35" si="8">LEN(B34)-LEN(SUBSTITUTE(B34,",",""))+1</f>
         <v>12</v>
@@ -2833,7 +2845,7 @@
         <v>Resistor - 12x 100k</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
         <f t="shared" si="8"/>
         <v>4</v>
@@ -2881,7 +2893,7 @@
         <v>Resistor - 4x 160</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
@@ -2901,7 +2913,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
         <v>1</v>
       </c>
@@ -2950,7 +2962,7 @@
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="40" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
         <v>1</v>
       </c>
@@ -2995,7 +3007,7 @@
         <v>1x 1-Bar MAP sensor</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22">
         <v>2</v>
       </c>
@@ -3042,7 +3054,7 @@
         <v>2x TC4424EPA</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
         <v>3</v>
       </c>
@@ -3083,7 +3095,7 @@
         <v>3x IC Socket</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
       <c r="B41" s="4"/>
       <c r="C41" s="3"/>
@@ -3103,7 +3115,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18">
         <v>0</v>
       </c>
@@ -3132,7 +3144,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
       <c r="B43" s="4"/>
       <c r="C43" s="3"/>
@@ -3152,7 +3164,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="4" t="s">
         <v>79</v>
@@ -3174,7 +3186,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18">
         <v>1</v>
       </c>
@@ -3211,7 +3223,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
         <v>1</v>
       </c>
@@ -3237,7 +3249,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="4"/>
       <c r="C47" s="3"/>
@@ -3256,14 +3268,20 @@
       </c>
       <c r="M47" s="12">
         <f>SUM(M2:M46)</f>
-        <v>92.298000000000002</v>
+        <v>92.138000000000005</v>
       </c>
       <c r="N47" s="11" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P47"/>
+  <autoFilter ref="A1:P47">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="N"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="J47:K47"/>
   </mergeCells>
@@ -3273,7 +3291,7 @@
     <hyperlink ref="K14" r:id="rId2"/>
     <hyperlink ref="K18" r:id="rId3"/>
     <hyperlink ref="K28" r:id="rId4" display="10.0KXBK-ND"/>
-    <hyperlink ref="K32" r:id="rId5"/>
+    <hyperlink ref="K32" r:id="rId5" display="985-1047-1-ND"/>
     <hyperlink ref="K33" r:id="rId6"/>
     <hyperlink ref="K34" r:id="rId7"/>
     <hyperlink ref="K38" r:id="rId8"/>

</xml_diff>

<commit_message>
Added Mouser part numbers to v0.3 BOM
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.3/v0.3.2_bom.xlsx
+++ b/reference/hardware/v0.3/v0.3.2_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full Kit" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,13 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2 Channel'!$A$1:$P$44</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Full Kit'!$A$1:$P$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Full Kit'!$A$1:$P$44</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +37,7 @@
     <author>Josh Stewart</author>
   </authors>
   <commentList>
-    <comment ref="B32" authorId="0">
+    <comment ref="B29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1411,13 +1414,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1483,7 +1486,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -1507,7 +1510,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
@@ -1549,7 +1552,7 @@
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4" t="str">
-        <f t="shared" ref="O3:O45" si="1">IF(NOT(K3=""),A3&amp;","&amp;K3,"")</f>
+        <f t="shared" ref="O3:O42" si="1">IF(NOT(K3=""),A3&amp;","&amp;K3,"")</f>
         <v>1,399-3654-ND</v>
       </c>
       <c r="P3" t="str">
@@ -1557,7 +1560,7 @@
         <v>Capacitor - 1x 10uF</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <f>LEN(B4)-LEN(SUBSTITUTE(B4,",",""))+1</f>
         <v>5</v>
@@ -1607,7 +1610,7 @@
         <v>Capacitor - 5x 0.22uF</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
         <v>7</v>
@@ -1657,7 +1660,7 @@
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
         <v>1</v>
@@ -1707,7 +1710,7 @@
         <v>Capacitor - 1x 47uF</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <f t="shared" ref="A7:A9" si="3">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
         <v>1</v>
@@ -1757,7 +1760,7 @@
         <v>Capacitor - 1x 0.33uF</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -1807,7 +1810,7 @@
         <v>Capacitor - 1x 0.01uF</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -1857,7 +1860,7 @@
         <v>Capacitor - 3x 1uF</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
         <v>1</v>
@@ -1905,7 +1908,7 @@
         <v>Capacitor - 1x 4.7nF</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -1925,477 +1928,507 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+    <row r="12" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20">
+        <f>LEN(B12)-LEN(SUBSTITUTE(B12,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0.34</v>
+      </c>
+      <c r="M12" s="6">
+        <f>L12*A12</f>
+        <v>0.34</v>
+      </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="40" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>1,1N5919BGOS-ND</v>
+      </c>
+      <c r="P12" t="str">
+        <f>"Diode - " &amp;A12&amp;"x "&amp;C12</f>
+        <v>Diode - 1x 1N5919BG Zener</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>22</v>
+        <v>151</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="J13" s="7" t="s">
-        <v>25</v>
+      <c r="J13" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L13" s="5">
-        <v>0.34</v>
+        <v>0.39</v>
       </c>
       <c r="M13" s="6">
         <f>L13*A13</f>
-        <v>0.34</v>
+        <v>4.68</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>1,1N5919BGOS-ND</v>
+        <v>12,1N5818-TPCT-ND</v>
       </c>
       <c r="P13" t="str">
-        <f>"Diode - " &amp;A13&amp;"x "&amp;C13</f>
-        <v>Diode - 1x 1N5919BG Zener</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="40" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="P13:P15" si="4">"Diode - " &amp;A13&amp;"x "&amp;C13</f>
+        <v>Diode - 12x 1N5818-TP Schottky</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>151</v>
+        <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="3">
-        <v>18</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="J14" s="3"/>
       <c r="K14" s="2" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="L14" s="5">
-        <v>0.39</v>
+        <v>0.47</v>
       </c>
       <c r="M14" s="6">
         <f>L14*A14</f>
-        <v>4.68</v>
+        <v>3.76</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>12,1N5818-TPCT-ND</v>
+        <v>8,160-1139-ND</v>
       </c>
       <c r="P14" t="str">
-        <f t="shared" ref="P14:P16" si="4">"Diode - " &amp;A14&amp;"x "&amp;C14</f>
-        <v>Diode - 12x 1N5818-TP Schottky</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>Diode - 8x LED-Red</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>117</v>
+        <v>33</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="G15" s="3">
+        <v>13</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="I15" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="J15" s="3"/>
+        <v>192</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="K15" s="2" t="s">
-        <v>118</v>
+        <v>35</v>
       </c>
       <c r="L15" s="5">
-        <v>0.47</v>
+        <v>0.11</v>
       </c>
       <c r="M15" s="6">
         <f>L15*A15</f>
-        <v>3.76</v>
+        <v>0.44</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>8,160-1139-ND</v>
+        <v>4,1N4004-TPMSCT-ND</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="4"/>
-        <v>Diode - 8x LED-Red</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="40" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
-        <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
-        <v>4</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>Diode - 4x 1N4004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="3">
-        <v>13</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L16" s="5">
-        <v>0.11</v>
-      </c>
-      <c r="M16" s="6">
-        <f>L16*A16</f>
-        <v>0.44</v>
-      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>4,1N4004-TPMSCT-ND</v>
+        <v/>
       </c>
       <c r="P16" t="str">
-        <f t="shared" si="4"/>
-        <v>Diode - 4x 1N4004</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+        <f t="shared" ref="P16:P37" si="5">A16&amp;"x "&amp;C16</f>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="M17" s="6">
+        <f>L17*A17</f>
+        <v>0.72</v>
+      </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1,P7307-ND</v>
       </c>
       <c r="P17" t="str">
-        <f t="shared" ref="P17:P40" si="5">A17&amp;"x "&amp;C17</f>
-        <v xml:space="preserve">x </v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
-        <v>1</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>38</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>1x Surge Protection</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="3">
-        <v>1</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L18" s="5">
-        <v>0.72</v>
-      </c>
-      <c r="M18" s="6">
-        <f>L18*A18</f>
-        <v>0.72</v>
-      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>1,P7307-ND</v>
+        <v/>
       </c>
       <c r="P18" t="str">
         <f t="shared" si="5"/>
-        <v>1x Surge Protection</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>14</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="4"/>
+      <c r="H19" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="M19" s="6">
+        <f>L19*A19</f>
+        <v>5.6280000000000001</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="O19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>14,ED2561-ND</v>
       </c>
       <c r="P19" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">x </v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+        <f>A19&amp;"x "&amp;C19</f>
+        <v>14x Dual Terminal Block</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
-        <v>130</v>
-      </c>
+      <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>133</v>
-      </c>
+      <c r="J20" s="3"/>
       <c r="K20" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="L20" s="3">
-        <v>0.40200000000000002</v>
+        <v>106</v>
+      </c>
+      <c r="L20" s="5">
+        <v>0.1</v>
       </c>
       <c r="M20" s="6">
         <f>L20*A20</f>
-        <v>5.6280000000000001</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>134</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="N20" s="4"/>
       <c r="O20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>14,ED2561-ND</v>
+        <v>5,3M9580-ND</v>
       </c>
       <c r="P20" t="str">
-        <f>A20&amp;"x "&amp;C20</f>
-        <v>14x Dual Terminal Block</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>5x Jumper</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>5</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="I21" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="J21" s="3"/>
+      <c r="J21" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="K21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L21" s="5">
-        <v>0.1</v>
+        <v>122</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0.56000000000000005</v>
       </c>
       <c r="M21" s="6">
         <f>L21*A21</f>
-        <v>0.5</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>5,3M9580-ND</v>
+        <v>5,S1012EC-40-ND</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" si="5"/>
-        <v>5x Jumper</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
-        <v>5</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>125</v>
-      </c>
+        <v>5x 40 POS 0.100 Pin Header</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="3">
-        <v>1</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L22" s="6">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="M22" s="6">
-        <f>L22*A22</f>
-        <v>2.8000000000000003</v>
-      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="6"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>5,S1012EC-40-ND</v>
+        <v/>
       </c>
       <c r="P22" t="str">
         <f t="shared" si="5"/>
-        <v>5x 40 POS 0.100 Pin Header</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20">
+        <f>LEN(B23)-LEN(SUBSTITUTE(B23,",",""))+1</f>
+        <v>8</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="6"/>
+      <c r="G23" s="3">
+        <v>8</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L23" s="6">
+        <v>1.51</v>
+      </c>
+      <c r="M23" s="6">
+        <f>L23*A23</f>
+        <v>12.08</v>
+      </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>8,497-5896-5-ND</v>
       </c>
       <c r="P23" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">x </v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>8x 62A MOSFET N-CH</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
@@ -2408,767 +2441,756 @@
       <c r="J24" s="3"/>
       <c r="K24" s="2"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="6"/>
+      <c r="M24" s="3"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P24" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">x </v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <f>LEN(B25)-LEN(SUBSTITUTE(B25,",",""))+1</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>114</v>
+        <v>194</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>144</v>
+        <v>44</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>74</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>192</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>105</v>
+        <v>46</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L25" s="6">
-        <v>1.51</v>
+        <v>195</v>
+      </c>
+      <c r="L25" s="5">
+        <v>0.08</v>
       </c>
       <c r="M25" s="6">
-        <f>L25*A25</f>
-        <v>12.08</v>
+        <f t="shared" ref="M25:M32" si="6">L25*A25</f>
+        <v>0.24</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>8,497-5896-5-ND</v>
+        <v>3,10KQBK-ND</v>
       </c>
       <c r="P25" t="str">
-        <f t="shared" si="5"/>
-        <v>8x 62A MOSFET N-CH</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+        <f>"Resistor - " &amp; A25&amp;"x "&amp;C25</f>
+        <v>Resistor - 3x 10k</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
+        <f>LEN(B26)-LEN(SUBSTITUTE(B26,",",""))+1</f>
+        <v>13</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
+      <c r="G26" s="3">
+        <v>32</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="M26" s="6">
+        <f t="shared" si="6"/>
+        <v>0.78</v>
+      </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+        <v>13,1.00KXBK-ND</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" ref="P26:P32" si="7">"Resistor - " &amp; A26&amp;"x "&amp;C26</f>
+        <v>Resistor - 13x 1k</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
+        <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
+        <v>8</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="14">
+        <v>680</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="4"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="J27" s="7"/>
+      <c r="K27" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="L27" s="15">
+        <v>0.22</v>
+      </c>
+      <c r="M27" s="6">
+        <f t="shared" si="6"/>
+        <v>1.76</v>
+      </c>
+      <c r="N27" s="13" t="s">
+        <v>121</v>
+      </c>
       <c r="O27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>8,A105963CT-ND</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 8x 680</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <f>LEN(B28)-LEN(SUBSTITUTE(B28,",",""))+1</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>44</v>
+        <v>190</v>
+      </c>
+      <c r="C28" s="3">
+        <v>470</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>196</v>
+        <v>51</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="J28" s="3" t="s">
-        <v>46</v>
+      <c r="J28" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>195</v>
+        <v>54</v>
       </c>
       <c r="L28" s="5">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="M28" s="6">
-        <f t="shared" ref="M28:M35" si="6">L28*A28</f>
-        <v>0.24</v>
+        <f t="shared" si="6"/>
+        <v>0.66</v>
       </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>3,10KQBK-ND</v>
+        <v>6,RNF14FTD470RCT-ND</v>
       </c>
       <c r="P28" t="str">
-        <f>"Resistor - " &amp; A28&amp;"x "&amp;C28</f>
-        <v>Resistor - 3x 10k</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>Resistor - 6x 470</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
-        <f>LEN(B29)-LEN(SUBSTITUTE(B29,",",""))+1</f>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>198</v>
+        <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="3"/>
+        <v>200</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>45</v>
+        <v>201</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>192</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>49</v>
+        <v>202</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>50</v>
+        <v>199</v>
       </c>
       <c r="L29" s="5">
-        <v>0.06</v>
+        <v>1.92</v>
       </c>
       <c r="M29" s="6">
         <f t="shared" si="6"/>
-        <v>0.78</v>
+        <v>3.84</v>
       </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>13,1.00KXBK-ND</v>
+        <v>2,PPC2.49KXCT-ND</v>
       </c>
       <c r="P29" t="str">
-        <f t="shared" ref="P29:P35" si="7">"Resistor - " &amp; A29&amp;"x "&amp;C29</f>
-        <v>Resistor - 13x 1k</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>Resistor - 2x 0.1% 2.49k</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
-        <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
-        <v>8</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" s="14">
-        <v>680</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>167</v>
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="I30" s="14" t="s">
+      <c r="F30" s="3"/>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I30" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="J30" s="7"/>
+      <c r="J30" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="K30" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="L30" s="15">
-        <v>0.22</v>
+        <v>62</v>
+      </c>
+      <c r="L30" s="5">
+        <v>0.3</v>
       </c>
       <c r="M30" s="6">
         <f t="shared" si="6"/>
-        <v>1.76</v>
-      </c>
-      <c r="N30" s="13" t="s">
-        <v>121</v>
+        <v>0.3</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="O30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>8,A105963CT-ND</v>
+        <v>1,3.9KADCT-ND</v>
       </c>
       <c r="P30" t="str">
         <f t="shared" si="7"/>
-        <v>Resistor - 8x 680</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="40" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>Resistor - 1x 0.1% 3.9k</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
-        <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
-        <v>6</v>
+        <f t="shared" ref="A31:A32" si="8">LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
+        <v>12</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C31" s="3">
-        <v>470</v>
+        <v>120</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="J31" s="7" t="s">
-        <v>53</v>
+      <c r="J31" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="L31" s="5">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="M31" s="6">
         <f t="shared" si="6"/>
-        <v>0.66</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="N31" s="4"/>
       <c r="O31" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>6,RNF14FTD470RCT-ND</v>
+        <v>12,100KXBK-ND</v>
       </c>
       <c r="P31" t="str">
         <f t="shared" si="7"/>
-        <v>Resistor - 6x 470</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>Resistor - 12x 100k</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>4</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>149</v>
+        <v>85</v>
+      </c>
+      <c r="C32" s="3">
+        <v>160</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>201</v>
+        <v>45</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>192</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>202</v>
+        <v>68</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>199</v>
+        <v>69</v>
       </c>
       <c r="L32" s="5">
-        <v>1.92</v>
+        <v>0.27</v>
       </c>
       <c r="M32" s="6">
         <f t="shared" si="6"/>
-        <v>3.84</v>
+        <v>1.08</v>
       </c>
       <c r="N32" s="4"/>
       <c r="O32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>2,PPC2.49KXCT-ND</v>
+        <v>4,160YCT-ND</v>
       </c>
       <c r="P32" t="str">
         <f t="shared" si="7"/>
-        <v>Resistor - 2x 0.1% 2.49k</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20">
-        <v>1</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>Resistor - 4x 160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="3">
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="20">
         <v>1</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L33" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="M33" s="6">
-        <f t="shared" si="6"/>
-        <v>0.3</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="O33" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>1,3.9KADCT-ND</v>
-      </c>
-      <c r="P33" t="str">
-        <f t="shared" si="7"/>
-        <v>Resistor - 1x 0.1% 3.9k</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20">
-        <f t="shared" ref="A34:A35" si="8">LEN(B34)-LEN(SUBSTITUTE(B34,",",""))+1</f>
-        <v>12</v>
-      </c>
       <c r="B34" s="4" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>192</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L34" s="5">
-        <v>0.1</v>
+        <v>1.68</v>
       </c>
       <c r="M34" s="6">
-        <f t="shared" si="6"/>
-        <v>1.2000000000000002</v>
+        <f>L34*A34</f>
+        <v>1.68</v>
       </c>
       <c r="N34" s="4"/>
       <c r="O34" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>12,100KXBK-ND</v>
+        <v>1,LM2940T-5.0/NOPB</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" si="7"/>
-        <v>Resistor - 12x 100k</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>1x LM2940T-5.0/NOPB</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
-        <f t="shared" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="3">
-        <v>160</v>
+        <v>95</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="3"/>
+        <v>94</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>68</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
       <c r="K35" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="L35" s="5">
-        <v>0.27</v>
+        <v>92</v>
+      </c>
+      <c r="L35" s="6">
+        <v>15.41</v>
       </c>
       <c r="M35" s="6">
-        <f t="shared" si="6"/>
-        <v>1.08</v>
+        <f>L35*A35</f>
+        <v>15.41</v>
       </c>
       <c r="N35" s="4"/>
       <c r="O35" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>4,160YCT-ND</v>
+        <v>1,MPX4250AP-ND</v>
       </c>
       <c r="P35" t="str">
-        <f t="shared" si="7"/>
-        <v>Resistor - 4x 160</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="4"/>
+        <f t="shared" si="5"/>
+        <v>1x 1-Bar MAP sensor</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22">
+        <v>2</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14">
+        <v>2</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="L36" s="23">
+        <v>2.92</v>
+      </c>
+      <c r="M36" s="6">
+        <f>L36*A36</f>
+        <v>5.84</v>
+      </c>
+      <c r="N36" s="13"/>
       <c r="O36" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2,TC4424EPA-ND</v>
+      </c>
+      <c r="P36" t="str">
+        <f t="shared" si="5"/>
+        <v>2x TC4424EPA</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
-        <v>1</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>70</v>
+        <v>3</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>74</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="3">
-        <v>2</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>75</v>
-      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
       <c r="I37" s="3" t="s">
         <v>192</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L37" s="5">
-        <v>1.68</v>
+        <v>96</v>
+      </c>
+      <c r="L37" s="6">
+        <v>0.5</v>
       </c>
       <c r="M37" s="6">
         <f>L37*A37</f>
-        <v>1.68</v>
+        <v>1.5</v>
       </c>
       <c r="N37" s="4"/>
       <c r="O37" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>1,LM2940T-5.0/NOPB</v>
+        <v>3,AE10011-ND</v>
       </c>
       <c r="P37" t="str">
         <f t="shared" si="5"/>
-        <v>1x LM2940T-5.0/NOPB</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="40" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="20">
+        <v>3x IC Socket</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="18">
+        <v>0</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3">
         <v>1</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3">
-        <v>1</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L38" s="6">
-        <v>15.41</v>
-      </c>
-      <c r="M38" s="6">
-        <f>L38*A38</f>
-        <v>15.41</v>
-      </c>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>1,MPX4250AP-ND</v>
-      </c>
-      <c r="P38" t="str">
-        <f t="shared" si="5"/>
-        <v>1x 1-Bar MAP sensor</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22">
-        <v>2</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14">
-        <v>2</v>
-      </c>
-      <c r="H39" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="L39" s="23">
-        <v>2.92</v>
-      </c>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="6"/>
       <c r="M39" s="6">
         <f>L39*A39</f>
-        <v>5.84</v>
-      </c>
-      <c r="N39" s="13"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="11"/>
       <c r="O39" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>2,TC4424EPA-ND</v>
-      </c>
-      <c r="P39" t="str">
-        <f t="shared" si="5"/>
-        <v>2x TC4424EPA</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="20">
-        <v>3</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>146</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="L40" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="M40" s="6">
-        <f>L40*A40</f>
-        <v>1.5</v>
-      </c>
-      <c r="N40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
       <c r="O40" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>3,AE10011-ND</v>
-      </c>
-      <c r="P40" t="str">
-        <f t="shared" si="5"/>
-        <v>3x IC Socket</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
-      <c r="B41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="4"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="9"/>
       <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="10"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="4"/>
       <c r="K41" s="3"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="4"/>
       <c r="O41" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="3"/>
+        <v>116</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3">
         <v>1</v>
       </c>
-      <c r="H42" s="3"/>
+      <c r="H42" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="6"/>
+      <c r="J42" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K42" s="3"/>
+      <c r="L42" s="6">
+        <v>15</v>
+      </c>
       <c r="M42" s="6">
         <f>L42*A42</f>
-        <v>0</v>
-      </c>
-      <c r="N42" s="11"/>
+        <v>15</v>
+      </c>
+      <c r="N42" s="4"/>
       <c r="O42" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="4"/>
+    <row r="43" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18">
+        <v>1</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L43" s="3">
+        <v>61.65</v>
+      </c>
+      <c r="M43" s="6"/>
+      <c r="N43" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
-      <c r="B44" s="4" t="s">
-        <v>79</v>
-      </c>
+      <c r="B44" s="4"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -3176,131 +3198,42 @@
       <c r="G44" s="9"/>
       <c r="H44" s="4"/>
       <c r="I44" s="9"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18">
-        <v>1</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3">
-        <v>1</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K45" s="3"/>
-      <c r="L45" s="6">
-        <v>15</v>
-      </c>
-      <c r="M45" s="6">
-        <f>L45*A45</f>
-        <v>15</v>
-      </c>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18">
-        <v>1</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="L46" s="3">
-        <v>61.65</v>
-      </c>
-      <c r="M46" s="6"/>
-      <c r="N46" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="27" t="s">
+      <c r="J44" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="K47" s="28"/>
-      <c r="L47" s="1" t="s">
+      <c r="K44" s="28"/>
+      <c r="L44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="M47" s="12">
-        <f>SUM(M2:M46)</f>
+      <c r="M44" s="12">
+        <f>SUM(M2:M43)</f>
         <v>92.138000000000005</v>
       </c>
-      <c r="N47" s="11" t="s">
+      <c r="N44" s="11" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P47">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="N"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:P44"/>
   <mergeCells count="1">
-    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J44:K44"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K6" r:id="rId1" display="478-1910-ND"/>
-    <hyperlink ref="K14" r:id="rId2"/>
-    <hyperlink ref="K18" r:id="rId3"/>
-    <hyperlink ref="K28" r:id="rId4" display="10.0KXBK-ND"/>
-    <hyperlink ref="K32" r:id="rId5" display="985-1047-1-ND"/>
-    <hyperlink ref="K33" r:id="rId6"/>
-    <hyperlink ref="K34" r:id="rId7"/>
-    <hyperlink ref="K38" r:id="rId8"/>
+    <hyperlink ref="K13" r:id="rId2"/>
+    <hyperlink ref="K17" r:id="rId3"/>
+    <hyperlink ref="K25" r:id="rId4" display="10.0KXBK-ND"/>
+    <hyperlink ref="K29" r:id="rId5" display="985-1047-1-ND"/>
+    <hyperlink ref="K30" r:id="rId6"/>
+    <hyperlink ref="K31" r:id="rId7"/>
+    <hyperlink ref="K35" r:id="rId8"/>
     <hyperlink ref="K3" r:id="rId9" display="478-1842-ND"/>
     <hyperlink ref="K7" r:id="rId10" display="445-5312-ND"/>
     <hyperlink ref="K8" r:id="rId11" display="399-4148-ND"/>
   </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="35" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>

</xml_diff>